<commit_message>
Change to decay figure source
</commit_message>
<xml_diff>
--- a/source/habitat_quality/HQ-decay-functions-chart.xlsx
+++ b/source/habitat_quality/HQ-decay-functions-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddenu\Workspace\NatCap\Repositories\invest.users-guide\source\habitat_quality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4AAFB98-05F5-4375-BFF8-0A72E69A7CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE8EB16-0CA7-41F1-B5BD-03FAD3D39027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{350C4C21-B092-4F87-8388-43652A6CC636}"/>
   </bookViews>
@@ -4599,7 +4599,7 @@
   <dimension ref="A1:C507"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N514" sqref="N514"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Updating figure png and source xlsx
</commit_message>
<xml_diff>
--- a/source/habitat_quality/HQ-decay-functions-chart.xlsx
+++ b/source/habitat_quality/HQ-decay-functions-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddenu\Workspace\NatCap\Repositories\invest.users-guide\source\habitat_quality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE8EB16-0CA7-41F1-B5BD-03FAD3D39027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21BBF9B-A4CE-49EF-8256-BC158A88B379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{350C4C21-B092-4F87-8388-43652A6CC636}"/>
   </bookViews>
@@ -106,10 +106,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="104"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="4"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -121,9 +121,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.10875453218337527"/>
-          <c:y val="3.2151987531380981E-2"/>
+          <c:y val="0.11128873279329295"/>
           <c:w val="0.84915951552746605"/>
-          <c:h val="0.83806123285035539"/>
+          <c:h val="0.75892445099038874"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -138,9 +138,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:shade val="53000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -789,9 +787,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:shade val="76000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1440,7 +1436,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2090,7 +2086,7 @@
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2">
-                  <a:tint val="77000"/>
+                  <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2740,8 +2736,8 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:tint val="54000"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -3428,7 +3424,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -3441,8 +3437,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
-                  <a:t>Max Distance of Threat (m)</a:t>
+                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:t>Distance (m)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3460,7 +3456,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -3498,7 +3494,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3545,13 +3541,27 @@
               <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
+                      <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      </a:sysClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3559,13 +3569,50 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
                   <a:t>i</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" b="1" baseline="-25000"/>
+                  <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
                   <a:t>rxy</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US" sz="1400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3581,13 +3628,27 @@
             <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
+                    <a:sysClr val="windowText" lastClr="000000">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    </a:sysClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -3620,7 +3681,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3653,8 +3714,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.81332905543004064"/>
-          <c:y val="0.21592901982698223"/>
+          <c:x val="0.75979750098430088"/>
+          <c:y val="0.27603863366000114"/>
           <c:w val="0.12186783952515273"/>
           <c:h val="0.29964984943571765"/>
         </c:manualLayout>
@@ -3721,7 +3782,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1100" baseline="0"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -3731,12 +3792,44 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="15">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -4260,16 +4353,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>33338</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>11113</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>52388</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4297,6 +4390,97 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.68476</cdr:x>
+      <cdr:y>0.22915</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95093</cdr:x>
+      <cdr:y>0.27746</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56E3EF6C-9191-2B67-5565-32D5B86B7E2F}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4386262" y="1213541"/>
+          <a:ext cx="1704974" cy="255840"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>Max Distance of Threat</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.27881</cdr:x>
+      <cdr:y>0.02878</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.72342</cdr:x>
+      <cdr:y>0.10791</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68195C36-7F10-5DD9-9ED5-AE01B85E3EF6}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1785935" y="152400"/>
+          <a:ext cx="2847975" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1"/>
+            <a:t>Exponential Decay of Threats</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4598,8 +4782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0294C04-675B-44C3-B97B-6F83172E938E}">
   <dimension ref="A1:C507"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4639,7 +4823,7 @@
         <v>50</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C23" si="0">EXP(-(2.99/A3)*B3)</f>
+        <f t="shared" ref="C3:C22" si="0">EXP(-(2.99/A3)*B3)</f>
         <v>0.86113843801970102</v>
       </c>
     </row>
@@ -5759,7 +5943,7 @@
         <v>0</v>
       </c>
       <c r="C103">
-        <f t="shared" ref="C74:C132" si="1">EXP(-(2.99/A103)*B103)</f>
+        <f t="shared" ref="C103:C105" si="1">EXP(-(2.99/A103)*B103)</f>
         <v>1</v>
       </c>
     </row>
@@ -5795,7 +5979,7 @@
         <v>150</v>
       </c>
       <c r="C106">
-        <f t="shared" ref="C106:C169" si="2">EXP(-(2.99/A106)*B106)</f>
+        <f t="shared" ref="C106:C143" si="2">EXP(-(2.99/A106)*B106)</f>
         <v>0.79911533056228934</v>
       </c>
     </row>
@@ -6911,7 +7095,7 @@
         <v>0</v>
       </c>
       <c r="C204">
-        <f t="shared" ref="C170:C208" si="3">EXP(-(2.99/A204)*B204)</f>
+        <f t="shared" ref="C204:C206" si="3">EXP(-(2.99/A204)*B204)</f>
         <v>1</v>
       </c>
     </row>
@@ -6947,7 +7131,7 @@
         <v>150</v>
       </c>
       <c r="C207">
-        <f t="shared" ref="C207:C270" si="4">EXP(-(2.99/A207)*B207)</f>
+        <f t="shared" ref="C207:C264" si="4">EXP(-(2.99/A207)*B207)</f>
         <v>0.86113843801970102</v>
       </c>
     </row>
@@ -8083,7 +8267,7 @@
         <v>0</v>
       </c>
       <c r="C305">
-        <f t="shared" ref="C271:C307" si="5">EXP(-(2.99/A305)*B305)</f>
+        <f t="shared" ref="C305:C307" si="5">EXP(-(2.99/A305)*B305)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>